<commit_message>
Fixed error in connection spread sheet
</commit_message>
<xml_diff>
--- a/Connections_Tables.xlsx
+++ b/Connections_Tables.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12440" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="P1" sheetId="1" r:id="rId1"/>
@@ -185,7 +185,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -196,6 +196,12 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -269,7 +275,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -280,6 +286,7 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -566,21 +573,21 @@
       <selection activeCell="K33" sqref="K33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="24.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.26953125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="23.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.453125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.26953125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="23.81640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.453125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="19.7265625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.453125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="19.7265625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="10.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -594,7 +601,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -632,7 +639,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
@@ -670,7 +677,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A4">
         <f xml:space="preserve"> A3+2</f>
         <v>4</v>
@@ -709,7 +716,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A5">
         <f t="shared" ref="A5:A20" si="0" xml:space="preserve"> A4+2</f>
         <v>6</v>
@@ -730,7 +737,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A6">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -751,7 +758,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A7">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -772,7 +779,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A8">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -793,7 +800,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A9">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -814,7 +821,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A10">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -835,7 +842,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A11">
         <f t="shared" si="0"/>
         <v>18</v>
@@ -856,7 +863,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A12">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -877,7 +884,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A13">
         <f t="shared" si="0"/>
         <v>22</v>
@@ -889,7 +896,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A14">
         <f t="shared" si="0"/>
         <v>24</v>
@@ -901,7 +908,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A15">
         <f t="shared" si="0"/>
         <v>26</v>
@@ -913,7 +920,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A16">
         <f xml:space="preserve"> A15+2</f>
         <v>28</v>
@@ -925,7 +932,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17">
         <f t="shared" si="0"/>
         <v>30</v>
@@ -937,7 +944,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18">
         <f t="shared" si="0"/>
         <v>32</v>
@@ -949,7 +956,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19">
         <f xml:space="preserve"> A18+2</f>
         <v>34</v>
@@ -961,7 +968,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20">
         <f t="shared" si="0"/>
         <v>36</v>
@@ -973,12 +980,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>12</v>
       </c>
@@ -986,7 +993,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>1</v>
       </c>
@@ -997,7 +1004,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>2</v>
       </c>
@@ -1014,24 +1021,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K28"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K28" sqref="K28"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="19" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.453125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="19" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.42578125" customWidth="1"/>
+    <col min="6" max="6" width="11.1796875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.453125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.453125" customWidth="1"/>
     <col min="10" max="10" width="23" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1042,7 +1049,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>26</v>
       </c>
@@ -1071,7 +1078,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>4</v>
       </c>
@@ -1095,7 +1102,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4">
         <f>A3+2</f>
         <v>6</v>
@@ -1126,7 +1133,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A5">
         <f t="shared" ref="A5:A24" si="0">A4+2</f>
         <v>8</v>
@@ -1157,7 +1164,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -1188,7 +1195,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A7">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -1219,7 +1226,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A8">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -1250,7 +1257,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A9">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -1281,7 +1288,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A10">
         <f t="shared" si="0"/>
         <v>18</v>
@@ -1312,7 +1319,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A11">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -1343,7 +1350,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A12">
         <f t="shared" si="0"/>
         <v>22</v>
@@ -1374,7 +1381,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A13">
         <f t="shared" si="0"/>
         <v>24</v>
@@ -1405,7 +1412,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A14">
         <f t="shared" si="0"/>
         <v>26</v>
@@ -1436,16 +1443,16 @@
         <v>48</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A15">
         <f t="shared" si="0"/>
         <v>28</v>
       </c>
       <c r="B15" t="s">
-        <v>3</v>
-      </c>
-      <c r="C15" t="s">
-        <v>3</v>
+        <v>30</v>
+      </c>
+      <c r="C15" s="10" t="s">
+        <v>31</v>
       </c>
       <c r="E15">
         <f t="shared" si="1"/>
@@ -1467,7 +1474,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A16">
         <f t="shared" si="0"/>
         <v>30</v>
@@ -1498,7 +1505,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A17">
         <f t="shared" si="0"/>
         <v>32</v>
@@ -1529,7 +1536,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A18">
         <f t="shared" si="0"/>
         <v>34</v>
@@ -1560,7 +1567,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A19">
         <f t="shared" si="0"/>
         <v>36</v>
@@ -1582,15 +1589,15 @@
         <v>3</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A20">
         <f t="shared" si="0"/>
         <v>38</v>
       </c>
       <c r="B20" t="s">
-        <v>30</v>
-      </c>
-      <c r="C20" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C20" s="6" t="s">
         <v>31</v>
       </c>
       <c r="D20" s="6"/>
@@ -1605,7 +1612,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A21">
         <f t="shared" si="0"/>
         <v>40</v>
@@ -1627,7 +1634,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A22">
         <f t="shared" si="0"/>
         <v>42</v>
@@ -1648,7 +1655,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A23">
         <f t="shared" si="0"/>
         <v>44</v>
@@ -1670,7 +1677,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A24">
         <f t="shared" si="0"/>
         <v>46</v>
@@ -1692,7 +1699,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A25">
         <f>A24+2</f>
         <v>48</v>
@@ -1714,7 +1721,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.35">
       <c r="E26">
         <f t="shared" si="2"/>
         <v>55</v>
@@ -1726,7 +1733,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.35">
       <c r="E27">
         <f t="shared" si="2"/>
         <v>57</v>
@@ -1738,7 +1745,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.35">
       <c r="E28">
         <f t="shared" si="2"/>
         <v>59</v>
@@ -1760,31 +1767,31 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="N29" sqref="N29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="24.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.26953125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.453125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="19" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.42578125" customWidth="1"/>
+    <col min="6" max="6" width="11.1796875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.453125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.453125" customWidth="1"/>
     <col min="10" max="10" width="23" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="23.85546875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.453125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.26953125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="23.81640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10.453125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="19.7265625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="10.453125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="19.7265625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="10.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1798,7 +1805,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -1836,7 +1843,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1869,7 +1876,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A4">
         <f xml:space="preserve"> A3+2</f>
         <v>4</v>
@@ -1909,7 +1916,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A5">
         <f t="shared" ref="A5:A20" si="0" xml:space="preserve"> A4+2</f>
         <v>6</v>
@@ -1949,7 +1956,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A6">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -1989,7 +1996,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A7">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -2029,7 +2036,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A8">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -2069,7 +2076,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A9">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -2109,7 +2116,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A10">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -2149,7 +2156,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A11">
         <f t="shared" si="0"/>
         <v>18</v>
@@ -2189,7 +2196,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A12">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -2229,7 +2236,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A13">
         <f t="shared" si="0"/>
         <v>22</v>
@@ -2260,7 +2267,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A14">
         <f t="shared" si="0"/>
         <v>24</v>
@@ -2291,7 +2298,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A15">
         <f t="shared" si="0"/>
         <v>26</v>
@@ -2322,7 +2329,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A16">
         <f xml:space="preserve"> A15+2</f>
         <v>28</v>
@@ -2353,7 +2360,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A17">
         <f t="shared" si="0"/>
         <v>30</v>
@@ -2384,7 +2391,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A18">
         <f t="shared" si="0"/>
         <v>32</v>
@@ -2415,7 +2422,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A19">
         <f xml:space="preserve"> A18+2</f>
         <v>34</v>
@@ -2437,7 +2444,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A20">
         <f t="shared" si="0"/>
         <v>36</v>
@@ -2459,7 +2466,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>38</v>
       </c>
@@ -2483,7 +2490,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.35">
       <c r="E22">
         <v>47</v>
       </c>
@@ -2494,7 +2501,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.35">
       <c r="E23">
         <f>E22+2</f>
         <v>49</v>
@@ -2506,7 +2513,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.35">
       <c r="E24">
         <f t="shared" ref="E24:E28" si="2">E23+2</f>
         <v>51</v>
@@ -2518,7 +2525,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.35">
       <c r="E25">
         <f t="shared" si="2"/>
         <v>53</v>
@@ -2530,7 +2537,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.35">
       <c r="E26">
         <f t="shared" si="2"/>
         <v>55</v>
@@ -2542,7 +2549,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.35">
       <c r="E27">
         <f t="shared" si="2"/>
         <v>57</v>
@@ -2554,7 +2561,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.35">
       <c r="E28">
         <f t="shared" si="2"/>
         <v>59</v>
@@ -2566,7 +2573,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>22</v>
       </c>
@@ -2577,7 +2584,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>12</v>
       </c>
@@ -2603,7 +2610,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A33">
         <v>1</v>
       </c>
@@ -2632,7 +2639,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A34">
         <v>2</v>
       </c>

</xml_diff>

<commit_message>
Updated Connections list again
</commit_message>
<xml_diff>
--- a/Connections_Tables.xlsx
+++ b/Connections_Tables.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12440" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12440" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="P1" sheetId="1" r:id="rId1"/>
@@ -275,7 +275,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -287,6 +287,7 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1021,8 +1022,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I2" sqref="I2:K18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1098,8 +1100,8 @@
       <c r="J3" t="s">
         <v>35</v>
       </c>
-      <c r="K3" s="9" t="s">
-        <v>36</v>
+      <c r="K3" s="11" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.35">
@@ -1158,10 +1160,10 @@
         <v>3</v>
       </c>
       <c r="J5" t="s">
-        <v>3</v>
-      </c>
-      <c r="K5" t="s">
-        <v>3</v>
+        <v>35</v>
+      </c>
+      <c r="K5" s="7" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.35">
@@ -1191,8 +1193,8 @@
       <c r="J6" t="s">
         <v>44</v>
       </c>
-      <c r="K6" s="7" t="s">
-        <v>25</v>
+      <c r="K6" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.35">
@@ -1220,10 +1222,10 @@
         <v>5</v>
       </c>
       <c r="J7" t="s">
-        <v>3</v>
-      </c>
-      <c r="K7" s="6" t="s">
-        <v>3</v>
+        <v>35</v>
+      </c>
+      <c r="K7" s="7" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.35">
@@ -1253,8 +1255,8 @@
       <c r="J8" t="s">
         <v>43</v>
       </c>
-      <c r="K8" s="7" t="s">
-        <v>25</v>
+      <c r="K8" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.35">
@@ -1358,8 +1360,8 @@
       <c r="B12" t="s">
         <v>33</v>
       </c>
-      <c r="C12" s="9" t="s">
-        <v>36</v>
+      <c r="C12" s="11" t="s">
+        <v>25</v>
       </c>
       <c r="E12">
         <f t="shared" si="1"/>
@@ -1368,8 +1370,8 @@
       <c r="F12" t="s">
         <v>37</v>
       </c>
-      <c r="G12" s="7" t="s">
-        <v>25</v>
+      <c r="G12" s="1" t="s">
+        <v>10</v>
       </c>
       <c r="I12">
         <v>10</v>
@@ -1399,8 +1401,8 @@
       <c r="F13" t="s">
         <v>34</v>
       </c>
-      <c r="G13" s="7" t="s">
-        <v>25</v>
+      <c r="G13" s="1" t="s">
+        <v>10</v>
       </c>
       <c r="I13">
         <v>11</v>
@@ -1767,8 +1769,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O34"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N29" sqref="N29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N16" sqref="N16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1863,8 +1865,8 @@
       <c r="J3" t="s">
         <v>35</v>
       </c>
-      <c r="K3" s="9" t="s">
-        <v>36</v>
+      <c r="K3" s="11" t="s">
+        <v>25</v>
       </c>
       <c r="M3">
         <v>1</v>
@@ -1941,10 +1943,10 @@
         <v>3</v>
       </c>
       <c r="J5" t="s">
-        <v>3</v>
-      </c>
-      <c r="K5" t="s">
-        <v>3</v>
+        <v>35</v>
+      </c>
+      <c r="K5" s="7" t="s">
+        <v>25</v>
       </c>
       <c r="M5">
         <v>3</v>
@@ -1983,8 +1985,8 @@
       <c r="J6" t="s">
         <v>44</v>
       </c>
-      <c r="K6" s="7" t="s">
-        <v>25</v>
+      <c r="K6" s="1" t="s">
+        <v>10</v>
       </c>
       <c r="M6">
         <v>4</v>
@@ -2021,10 +2023,10 @@
         <v>5</v>
       </c>
       <c r="J7" t="s">
-        <v>3</v>
-      </c>
-      <c r="K7" s="6" t="s">
-        <v>3</v>
+        <v>35</v>
+      </c>
+      <c r="K7" s="7" t="s">
+        <v>25</v>
       </c>
       <c r="M7">
         <v>5</v>
@@ -2063,8 +2065,8 @@
       <c r="J8" t="s">
         <v>43</v>
       </c>
-      <c r="K8" s="7" t="s">
-        <v>25</v>
+      <c r="K8" s="1" t="s">
+        <v>10</v>
       </c>
       <c r="M8">
         <v>6</v>
@@ -2214,8 +2216,8 @@
       <c r="F12" t="s">
         <v>37</v>
       </c>
-      <c r="G12" s="7" t="s">
-        <v>25</v>
+      <c r="G12" s="1" t="s">
+        <v>10</v>
       </c>
       <c r="I12">
         <v>10</v>
@@ -2254,8 +2256,8 @@
       <c r="F13" t="s">
         <v>34</v>
       </c>
-      <c r="G13" s="7" t="s">
-        <v>25</v>
+      <c r="G13" s="1" t="s">
+        <v>10</v>
       </c>
       <c r="I13">
         <v>11</v>

</xml_diff>